<commit_message>
Add strings to relevant spreadsheets
</commit_message>
<xml_diff>
--- a/translations/RUS/admin-strings_RUS.xlsx
+++ b/translations/RUS/admin-strings_RUS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
   <si>
     <t>English</t>
   </si>
@@ -1170,13 +1170,68 @@
   </si>
   <si>
     <t>Чего ожидать в этом местоположении</t>
+  </si>
+  <si>
+    <t>Before</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Перед </t>
+  </si>
+  <si>
+    <t>During</t>
+  </si>
+  <si>
+    <t>В течение</t>
+  </si>
+  <si>
+    <t>After</t>
+  </si>
+  <si>
+    <t>После</t>
+  </si>
+  <si>
+    <t>What's Happened?</t>
+  </si>
+  <si>
+    <t>Что случилось?</t>
+  </si>
+  <si>
+    <t>What's the Worst?</t>
+  </si>
+  <si>
+    <t>Что хуже всего?</t>
+  </si>
+  <si>
+    <t>Cascadia Quake</t>
+  </si>
+  <si>
+    <t>Разлом Каскадия</t>
+  </si>
+  <si>
+    <t>Tsunami Zone</t>
+  </si>
+  <si>
+    <t>Зона цунами</t>
+  </si>
+  <si>
+    <t>If the dams failed</t>
+  </si>
+  <si>
+    <t>Если прорвало плотину</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1240,28 +1295,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1542,10 +1603,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B96"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92:B92"/>
+      <selection activeCell="A93" sqref="A93:B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="75.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2290,10 +2351,70 @@
         <v>183</v>
       </c>
     </row>
-    <row r="93" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="94" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="95" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="96" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="93" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>